<commit_message>
NBC model added, log updated
</commit_message>
<xml_diff>
--- a/DetailedLog.xlsx
+++ b/DetailedLog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tomas\4thYearSofDev\DataScience\DataScienceModuleGitHub\DataScienceModule\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E558E4E-5A54-4021-AFB4-E82694078E7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8E28DF8-4CB3-47C5-8AD4-FAFA6E76FB8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{F649E3DD-3891-45EF-9659-861F4028E8C6}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{F649E3DD-3891-45EF-9659-861F4028E8C6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="33">
   <si>
     <t>Date</t>
   </si>
@@ -117,6 +117,24 @@
   </si>
   <si>
     <t>Understanding the code, PythonDataSceicneHandbook</t>
+  </si>
+  <si>
+    <t>Example completed</t>
+  </si>
+  <si>
+    <t>Follow the example on my dataset</t>
+  </si>
+  <si>
+    <t>Followed Handbook on my own data, used model tunning to increase the accuracy by 2% by changing training, validation and testing size and by tunning hyperparameters</t>
+  </si>
+  <si>
+    <t>Highest model accuracy on test set is 79.2%, not great</t>
+  </si>
+  <si>
+    <t>Detail information in my portfolio</t>
+  </si>
+  <si>
+    <t>Modeling section for NBC</t>
   </si>
 </sst>
 </file>
@@ -217,7 +235,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -228,9 +246,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -239,6 +254,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -574,10 +595,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46F8E825-9A85-45B3-9061-C505070C3A75}">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -638,15 +659,15 @@
       </c>
     </row>
     <row r="3" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="7"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="6"/>
     </row>
     <row r="4" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
@@ -742,74 +763,167 @@
     </row>
     <row r="8" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
-        <v>45681</v>
+        <v>45680</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>26</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="4"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
+      <c r="E8" s="3">
+        <v>1</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="2">
+        <v>45680</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="7">
+        <v>2</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="2">
+        <v>45680</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="7">
+        <v>1</v>
+      </c>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
+      <c r="A11" s="7"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="4"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
+      <c r="A12" s="7"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="4"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
+      <c r="A13" s="7"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="4"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
+      <c r="A14" s="7"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" s="8"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" s="8"/>
+      <c r="B16" s="8"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" s="8"/>
+      <c r="B17" s="8"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" s="8"/>
+      <c r="B18" s="8"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="8"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" s="8"/>
+      <c r="B19" s="8"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="8"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" s="8"/>
+      <c r="B20" s="8"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="8"/>
+      <c r="G20" s="8"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" s="8"/>
+      <c r="B21" s="8"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="8"/>
+      <c r="G21" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
log updated, KNN R file added
</commit_message>
<xml_diff>
--- a/DetailedLog.xlsx
+++ b/DetailedLog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tomas\4thYearSofDev\DataScience\DataScienceModuleGitHub\DataScienceModule\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F331039C-08BC-4A0C-811E-14CC83B5CAA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{344C3C64-674A-4652-A846-B4D7A333FE73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{F649E3DD-3891-45EF-9659-861F4028E8C6}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="67">
   <si>
     <t>Date</t>
   </si>
@@ -195,6 +195,48 @@
   </si>
   <si>
     <t>Redid the SVM model with the new insights, and changing the columns to see if it improves accuracy</t>
+  </si>
+  <si>
+    <t>Start KNN research</t>
+  </si>
+  <si>
+    <t>Started research for the KNN model what what I want to achieve with it. Did a simple model with the famous iris dataset. Wanted to do it on a harder dataset so chose a wine dataset to predict the quality of the wine</t>
+  </si>
+  <si>
+    <t>Wine dataset downloaded in csv. Business objectives started</t>
+  </si>
+  <si>
+    <t>Train model KNN</t>
+  </si>
+  <si>
+    <t>Simple model trained</t>
+  </si>
+  <si>
+    <t>Poor accuracy of 51%</t>
+  </si>
+  <si>
+    <t>complete data visualisation</t>
+  </si>
+  <si>
+    <t>Data visualisation to give insights into the data</t>
+  </si>
+  <si>
+    <t>Produced 3 data visualisation graphs. Distribution, acidity by quality , content by quality</t>
+  </si>
+  <si>
+    <t>Improve model</t>
+  </si>
+  <si>
+    <t>Improve model by cleaning data, data cleaning, removing columns with no correlation, finding the best k value</t>
+  </si>
+  <si>
+    <t>Improved to 59% through tunning, still poor accuracy</t>
+  </si>
+  <si>
+    <t>Documentation on portfolio</t>
+  </si>
+  <si>
+    <t>Documentation on porfolio of process</t>
   </si>
 </sst>
 </file>
@@ -309,11 +351,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -658,10 +700,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46F8E825-9A85-45B3-9061-C505070C3A75}">
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:G31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -915,7 +957,7 @@
       </c>
     </row>
     <row r="12" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A12" s="6">
+      <c r="A12" s="5">
         <v>45688</v>
       </c>
       <c r="B12" s="4" t="s">
@@ -938,7 +980,7 @@
       </c>
     </row>
     <row r="13" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A13" s="6">
+      <c r="A13" s="5">
         <v>45691</v>
       </c>
       <c r="B13" s="4" t="s">
@@ -961,7 +1003,7 @@
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="6">
+      <c r="A14" s="5">
         <v>45691</v>
       </c>
       <c r="B14" s="4" t="s">
@@ -976,7 +1018,7 @@
       <c r="G14" s="4"/>
     </row>
     <row r="15" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A15" s="6">
+      <c r="A15" s="5">
         <v>45694</v>
       </c>
       <c r="B15" s="4" t="s">
@@ -999,7 +1041,7 @@
       </c>
     </row>
     <row r="16" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A16" s="6">
+      <c r="A16" s="5">
         <v>45695</v>
       </c>
       <c r="B16" s="4" t="s">
@@ -1018,7 +1060,7 @@
       <c r="G16" s="4"/>
     </row>
     <row r="17" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A17" s="6">
+      <c r="A17" s="5">
         <v>45702</v>
       </c>
       <c r="B17" s="4" t="s">
@@ -1039,7 +1081,7 @@
       <c r="G17" s="4"/>
     </row>
     <row r="18" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A18" s="6">
+      <c r="A18" s="5">
         <v>45703</v>
       </c>
       <c r="B18" s="4" t="s">
@@ -1060,7 +1102,7 @@
       <c r="G18" s="4"/>
     </row>
     <row r="19" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A19" s="6">
+      <c r="A19" s="5">
         <v>45703</v>
       </c>
       <c r="B19" s="4" t="s">
@@ -1076,25 +1118,183 @@
         <v>1</v>
       </c>
       <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="5"/>
-      <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
+      <c r="G19" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A20" s="5">
+        <v>45706</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E20" s="4">
+        <v>1</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" s="5"/>
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="5"/>
+      <c r="A21" s="5">
+        <v>45706</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E21" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A22" s="5">
+        <v>45706</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E22" s="4">
+        <v>1</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A23" s="5">
+        <v>45707</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E23" s="4">
+        <v>2</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="G23" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24" s="5">
+        <v>45707</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E24" s="4">
+        <v>3</v>
+      </c>
+      <c r="F24" s="4"/>
+      <c r="G24" s="4"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25" s="4"/>
+      <c r="B25" s="4"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
+      <c r="F25" s="4"/>
+      <c r="G25" s="4"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26" s="4"/>
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="4"/>
+      <c r="G26" s="4"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27" s="4"/>
+      <c r="B27" s="4"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="4"/>
+      <c r="F27" s="4"/>
+      <c r="G27" s="4"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A28" s="4"/>
+      <c r="B28" s="4"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="4"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="4"/>
+      <c r="G28" s="4"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A29" s="6"/>
+      <c r="B29" s="6"/>
+      <c r="C29" s="6"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="6"/>
+      <c r="G29" s="6"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A30" s="6"/>
+      <c r="B30" s="6"/>
+      <c r="C30" s="6"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="6"/>
+      <c r="F30" s="6"/>
+      <c r="G30" s="6"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A31" s="6"/>
+      <c r="B31" s="6"/>
+      <c r="C31" s="6"/>
+      <c r="D31" s="6"/>
+      <c r="E31" s="6"/>
+      <c r="F31" s="6"/>
+      <c r="G31" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
KNN R file finished, log updated
</commit_message>
<xml_diff>
--- a/DetailedLog.xlsx
+++ b/DetailedLog.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tomas\4thYearSofDev\DataScience\DataScienceModuleGitHub\DataScienceModule\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tomas\4thYearSofDev\DataScience\DataScienceModuleGitHub2\DataScienceModule\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{344C3C64-674A-4652-A846-B4D7A333FE73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A1FD6A4-7C9E-4C2A-A304-D5F2BD73AB18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{F649E3DD-3891-45EF-9659-861F4028E8C6}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="69">
   <si>
     <t>Date</t>
   </si>
@@ -237,6 +237,12 @@
   </si>
   <si>
     <t>Documentation on porfolio of process</t>
+  </si>
+  <si>
+    <t>references added</t>
+  </si>
+  <si>
+    <t>Start K means</t>
   </si>
 </sst>
 </file>
@@ -703,7 +709,7 @@
   <dimension ref="A1:G31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1010,7 +1016,7 @@
         <v>40</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
@@ -1025,7 +1031,7 @@
         <v>43</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="D15" s="4" t="s">
         <v>13</v>
@@ -1048,7 +1054,7 @@
         <v>46</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="D16" s="4" t="s">
         <v>13</v>
@@ -1230,8 +1236,12 @@
       <c r="E24" s="4">
         <v>3</v>
       </c>
-      <c r="F24" s="4"/>
-      <c r="G24" s="4"/>
+      <c r="F24" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="G24" s="4" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="4"/>

</xml_diff>

<commit_message>
Kmeans example completed, log updated
</commit_message>
<xml_diff>
--- a/DetailedLog.xlsx
+++ b/DetailedLog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tomas\4thYearSofDev\DataScience\DataScienceModuleGitHub2\DataScienceModule\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A1FD6A4-7C9E-4C2A-A304-D5F2BD73AB18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C0E6CF6-16D7-4ABA-8222-0E12C5450499}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{F649E3DD-3891-45EF-9659-861F4028E8C6}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="73">
   <si>
     <t>Date</t>
   </si>
@@ -243,6 +243,18 @@
   </si>
   <si>
     <t>Start K means</t>
+  </si>
+  <si>
+    <t>K mean python notebook example</t>
+  </si>
+  <si>
+    <t>completed</t>
+  </si>
+  <si>
+    <t>research project ideas</t>
+  </si>
+  <si>
+    <t>Find new dataset and perform basic k mean model</t>
   </si>
 </sst>
 </file>
@@ -708,8 +720,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46F8E825-9A85-45B3-9061-C505070C3A75}">
   <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1244,20 +1256,44 @@
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" s="4"/>
-      <c r="B25" s="4"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="4"/>
-      <c r="E25" s="4"/>
-      <c r="F25" s="4"/>
-      <c r="G25" s="4"/>
+      <c r="A25" s="5">
+        <v>45707</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E25" s="4">
+        <v>1</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="G25" s="4" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A26" s="4"/>
-      <c r="B26" s="4"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="4"/>
-      <c r="E26" s="4"/>
+      <c r="A26" s="5">
+        <v>45707</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E26" s="4">
+        <v>1</v>
+      </c>
       <c r="F26" s="4"/>
       <c r="G26" s="4"/>
     </row>

</xml_diff>

<commit_message>
log updated, KMC code added
</commit_message>
<xml_diff>
--- a/DetailedLog.xlsx
+++ b/DetailedLog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tomas\4thYearSofDev\DataScience\DataScienceModuleGitHub2\DataScienceModule\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C0E6CF6-16D7-4ABA-8222-0E12C5450499}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FFFF705-0D1A-4C0B-B36B-C97D81153953}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{F649E3DD-3891-45EF-9659-861F4028E8C6}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="81">
   <si>
     <t>Date</t>
   </si>
@@ -71,9 +71,6 @@
     <t>Continue adding rows and improve layout</t>
   </si>
   <si>
-    <t>Naive Bayes Classifier</t>
-  </si>
-  <si>
     <t>Understand Naive Bayes Classifier</t>
   </si>
   <si>
@@ -255,6 +252,33 @@
   </si>
   <si>
     <t>Find new dataset and perform basic k mean model</t>
+  </si>
+  <si>
+    <t>Used the same dataset as before for wine quality to see the the accuracy can be improved with this model, since I wasn’t too happy with the 59% accuracy with the KNN model</t>
+  </si>
+  <si>
+    <t>After attempting to do it with the wine dataset, it worked poorly and got low silhouette score so decided to do it on a defferent dataset</t>
+  </si>
+  <si>
+    <t>Found food nutrition dataset</t>
+  </si>
+  <si>
+    <t>do K mean clustering on new dataset</t>
+  </si>
+  <si>
+    <t>K means clustering done on new dataser, elbow method didn’t work to find best k so used silhoette method</t>
+  </si>
+  <si>
+    <t>improve</t>
+  </si>
+  <si>
+    <t>Did feature selection to focus on the most relevant columns to predict what clusters the foods are most/least in sugar, fiber, protein, etc</t>
+  </si>
+  <si>
+    <t>.26 silhoette score, resonable results but could be improved further</t>
+  </si>
+  <si>
+    <t>complete crisp-dm documentation for portfolio</t>
   </si>
 </sst>
 </file>
@@ -291,7 +315,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -314,48 +338,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color rgb="FFCCCCCC"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color rgb="FFCCCCCC"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FFCCCCCC"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color rgb="FFCCCCCC"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FFCCCCCC"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color rgb="FFCCCCCC"/>
-      </right>
-      <top style="medium">
-        <color rgb="FFCCCCCC"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FFCCCCCC"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -373,16 +360,7 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -718,10 +696,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46F8E825-9A85-45B3-9061-C505070C3A75}">
-  <dimension ref="A1:G31"/>
+  <dimension ref="A1:G35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -775,147 +753,159 @@
         <v>0.2</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="2">
+        <v>45674</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="9"/>
-    </row>
-    <row r="4" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="3">
+        <v>2</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="54" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
         <v>45674</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="3">
-        <v>2</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>14</v>
-      </c>
       <c r="G4" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="2">
+        <v>45675</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" ht="54" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="2">
-        <v>45674</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>18</v>
-      </c>
       <c r="C5" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E5" s="3">
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
-        <v>45675</v>
+        <v>45680</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E6" s="3">
-        <v>1</v>
+        <v>0.3</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
         <v>45680</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E7" s="3">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
         <v>45680</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E8" s="3">
-        <v>1</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="G8" s="3" t="s">
+      <c r="B8" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="4">
+        <v>2</v>
+      </c>
+      <c r="F8" s="4" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G8" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="2">
         <v>45680</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>9</v>
@@ -923,178 +913,176 @@
       <c r="E9" s="4">
         <v>2</v>
       </c>
-      <c r="F9" s="4" t="s">
-        <v>29</v>
-      </c>
+      <c r="F9" s="4"/>
       <c r="G9" s="4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="2">
-        <v>45680</v>
+        <v>45683</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E10" s="4">
+        <v>1</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A11" s="5">
+        <v>45688</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" s="4">
         <v>2</v>
       </c>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="2">
-        <v>45683</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E11" s="4">
-        <v>1</v>
-      </c>
       <c r="F11" s="4" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="5">
-        <v>45688</v>
+        <v>45691</v>
       </c>
       <c r="B12" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E12" s="4">
+        <v>1</v>
+      </c>
+      <c r="F12" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C12" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E12" s="4">
-        <v>2</v>
-      </c>
-      <c r="F12" s="4" t="s">
+      <c r="G12" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="G12" s="4" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="5">
         <v>45691</v>
       </c>
       <c r="B13" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+    </row>
+    <row r="14" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A14" s="5">
+        <v>45694</v>
+      </c>
+      <c r="B14" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="C13" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E13" s="4">
-        <v>1</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="G13" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="5">
-        <v>45691</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>40</v>
-      </c>
       <c r="C14" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
+        <v>15</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E14" s="4">
+        <v>3</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="15" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="5">
-        <v>45694</v>
+        <v>45695</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E15" s="4">
-        <v>3</v>
-      </c>
-      <c r="F15" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="G15" s="4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+    </row>
+    <row r="16" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A16" s="5">
-        <v>45695</v>
+        <v>45702</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>46</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E16" s="4">
-        <v>2</v>
-      </c>
-      <c r="F16" s="4"/>
+        <v>1</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>47</v>
+      </c>
       <c r="G16" s="4"/>
     </row>
-    <row r="17" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" s="5">
-        <v>45702</v>
+        <v>45703</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>13</v>
+        <v>49</v>
       </c>
       <c r="E17" s="4">
-        <v>1</v>
+        <v>0.3</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="G17" s="4"/>
     </row>
@@ -1103,133 +1091,135 @@
         <v>45703</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>50</v>
+        <v>12</v>
       </c>
       <c r="E18" s="4">
-        <v>0.3</v>
-      </c>
-      <c r="F18" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="G18" s="4"/>
-    </row>
-    <row r="19" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A19" s="5">
-        <v>45703</v>
+        <v>45706</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E19" s="4">
         <v>1</v>
       </c>
-      <c r="F19" s="4"/>
+      <c r="F19" s="4" t="s">
+        <v>54</v>
+      </c>
       <c r="G19" s="4" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="5">
         <v>45706</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E20" s="4">
-        <v>1</v>
+        <v>0.3</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A21" s="5">
         <v>45706</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E21" s="4">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A22" s="5">
-        <v>45706</v>
+        <v>45707</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E22" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="5">
         <v>45707</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E23" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
@@ -1237,101 +1227,129 @@
         <v>45707</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E24" s="4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="72" x14ac:dyDescent="0.3">
       <c r="A25" s="5">
         <v>45707</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E25" s="4">
         <v>1</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="G25" s="4" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+        <v>72</v>
+      </c>
+      <c r="G25" s="4"/>
+    </row>
+    <row r="26" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A26" s="5">
         <v>45707</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E26" s="4">
+        <v>2</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="G26" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A27" s="5">
+        <v>45709</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E27" s="4">
         <v>1</v>
       </c>
-      <c r="F26" s="4"/>
-      <c r="G26" s="4"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27" s="4"/>
-      <c r="B27" s="4"/>
-      <c r="C27" s="4"/>
-      <c r="D27" s="4"/>
-      <c r="E27" s="4"/>
       <c r="F27" s="4"/>
-      <c r="G27" s="4"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A28" s="4"/>
-      <c r="B28" s="4"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="4"/>
-      <c r="E28" s="4"/>
-      <c r="F28" s="4"/>
-      <c r="G28" s="4"/>
+      <c r="G27" s="4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A28" s="5">
+        <v>45709</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E28" s="4">
+        <v>1</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="G28" s="4" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" s="6"/>
-      <c r="B29" s="6"/>
-      <c r="C29" s="6"/>
-      <c r="D29" s="6"/>
-      <c r="E29" s="6"/>
-      <c r="F29" s="6"/>
-      <c r="G29" s="6"/>
+      <c r="A29" s="4"/>
+      <c r="B29" s="4"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="4"/>
+      <c r="G29" s="4"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" s="6"/>
-      <c r="B30" s="6"/>
-      <c r="C30" s="6"/>
-      <c r="D30" s="6"/>
-      <c r="E30" s="6"/>
-      <c r="F30" s="6"/>
-      <c r="G30" s="6"/>
+      <c r="A30" s="4"/>
+      <c r="B30" s="4"/>
+      <c r="C30" s="4"/>
+      <c r="D30" s="4"/>
+      <c r="E30" s="4"/>
+      <c r="F30" s="4"/>
+      <c r="G30" s="4"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="6"/>
@@ -1342,10 +1360,43 @@
       <c r="F31" s="6"/>
       <c r="G31" s="6"/>
     </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A32" s="6"/>
+      <c r="B32" s="6"/>
+      <c r="C32" s="6"/>
+      <c r="D32" s="6"/>
+      <c r="E32" s="6"/>
+      <c r="F32" s="6"/>
+      <c r="G32" s="6"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A33" s="6"/>
+      <c r="B33" s="6"/>
+      <c r="C33" s="6"/>
+      <c r="D33" s="6"/>
+      <c r="E33" s="6"/>
+      <c r="F33" s="6"/>
+      <c r="G33" s="6"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A34" s="6"/>
+      <c r="B34" s="6"/>
+      <c r="C34" s="6"/>
+      <c r="D34" s="6"/>
+      <c r="E34" s="6"/>
+      <c r="F34" s="6"/>
+      <c r="G34" s="6"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A35" s="6"/>
+      <c r="B35" s="6"/>
+      <c r="C35" s="6"/>
+      <c r="D35" s="6"/>
+      <c r="E35" s="6"/>
+      <c r="F35" s="6"/>
+      <c r="G35" s="6"/>
+    </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A3:G3"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Log updated, NN number example  added
</commit_message>
<xml_diff>
--- a/DetailedLog.xlsx
+++ b/DetailedLog.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tomas\4thYearSofDev\DataScience\DataScienceModuleGitHub2\DataScienceModule\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E5C8140-CA2A-4A8E-9871-45D44E66853F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60208F2B-C17A-4051-99A2-9ACB8123FD40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{F649E3DD-3891-45EF-9659-861F4028E8C6}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{F649E3DD-3891-45EF-9659-861F4028E8C6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="89">
   <si>
     <t>Date</t>
   </si>
@@ -98,9 +98,6 @@
     <t>Decide on what data to use the model</t>
   </si>
   <si>
-    <t>Performing business understanding and data understanding on the database, available on GitHub</t>
-  </si>
-  <si>
     <t>Added business understanding and data understanding to the portfolio</t>
   </si>
   <si>
@@ -285,13 +282,34 @@
   </si>
   <si>
     <t>Fixed issue with KNN model matrix not showing correct data</t>
+  </si>
+  <si>
+    <t>Performing business understanding and data understanding on the dataset, available on GitHub</t>
+  </si>
+  <si>
+    <t>Review Neural Network Notes</t>
+  </si>
+  <si>
+    <t>Focusing on Feedforward NN</t>
+  </si>
+  <si>
+    <t>Start NN projects</t>
+  </si>
+  <si>
+    <t>Start business undersatnding and data understanding for FNN</t>
+  </si>
+  <si>
+    <t>Following example : github.com/trekhleb. For using Tensorflow to predict writen numbers</t>
+  </si>
+  <si>
+    <t>Find a dataset to do my own training</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -311,6 +329,13 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -348,7 +373,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -359,13 +384,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -702,10 +728,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46F8E825-9A85-45B3-9061-C505070C3A75}">
-  <dimension ref="A1:G39"/>
+  <dimension ref="A1:I52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -816,7 +842,7 @@
         <v>45675</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>20</v>
+        <v>82</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>15</v>
@@ -828,10 +854,10 @@
         <v>1</v>
       </c>
       <c r="F5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" s="3" t="s">
         <v>21</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
@@ -839,7 +865,7 @@
         <v>45680</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>15</v>
@@ -851,10 +877,10 @@
         <v>0.3</v>
       </c>
       <c r="F6" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G6" s="3" t="s">
         <v>24</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -862,7 +888,7 @@
         <v>45680</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>15</v>
@@ -874,18 +900,18 @@
         <v>1</v>
       </c>
       <c r="F7" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G7" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="G7" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="8" spans="1:7" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
         <v>45680</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>15</v>
@@ -897,10 +923,10 @@
         <v>2</v>
       </c>
       <c r="F8" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G8" s="4" t="s">
         <v>28</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -908,7 +934,7 @@
         <v>45680</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>15</v>
@@ -921,7 +947,7 @@
       </c>
       <c r="F9" s="4"/>
       <c r="G9" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -929,7 +955,7 @@
         <v>45683</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>15</v>
@@ -941,18 +967,18 @@
         <v>1</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="27" x14ac:dyDescent="0.3">
       <c r="A11" s="5">
         <v>45688</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>15</v>
@@ -964,18 +990,18 @@
         <v>2</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="27" x14ac:dyDescent="0.3">
       <c r="A12" s="5">
         <v>45691</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>15</v>
@@ -987,10 +1013,10 @@
         <v>1</v>
       </c>
       <c r="F12" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="G12" s="4" t="s">
         <v>37</v>
-      </c>
-      <c r="G12" s="4" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
@@ -998,7 +1024,7 @@
         <v>45691</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>15</v>
@@ -1008,12 +1034,12 @@
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
     </row>
-    <row r="14" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" ht="27" x14ac:dyDescent="0.3">
       <c r="A14" s="5">
         <v>45694</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>15</v>
@@ -1025,18 +1051,18 @@
         <v>3</v>
       </c>
       <c r="F14" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="G14" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="G14" s="4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:7" ht="27" x14ac:dyDescent="0.3">
       <c r="A15" s="5">
         <v>45695</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>15</v>
@@ -1050,12 +1076,12 @@
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
     </row>
-    <row r="16" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" ht="40.200000000000003" x14ac:dyDescent="0.3">
       <c r="A16" s="5">
         <v>45702</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>15</v>
@@ -1067,37 +1093,37 @@
         <v>1</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G16" s="4"/>
     </row>
-    <row r="17" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" ht="27" x14ac:dyDescent="0.3">
       <c r="A17" s="5">
         <v>45703</v>
       </c>
       <c r="B17" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D17" s="4" t="s">
         <v>48</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>49</v>
       </c>
       <c r="E17" s="4">
         <v>0.3</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G17" s="4"/>
     </row>
-    <row r="18" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" ht="27" x14ac:dyDescent="0.3">
       <c r="A18" s="5">
         <v>45703</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>15</v>
@@ -1110,15 +1136,15 @@
       </c>
       <c r="F18" s="4"/>
       <c r="G18" s="4" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="53.4" x14ac:dyDescent="0.3">
       <c r="A19" s="5">
         <v>45706</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>15</v>
@@ -1130,18 +1156,18 @@
         <v>1</v>
       </c>
       <c r="F19" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="G19" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="G19" s="4" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="5">
         <v>45706</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>15</v>
@@ -1153,18 +1179,18 @@
         <v>0.3</v>
       </c>
       <c r="F20" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="G20" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="G20" s="4" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="21" spans="1:9" ht="40.200000000000003" x14ac:dyDescent="0.3">
       <c r="A21" s="5">
         <v>45706</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>15</v>
@@ -1176,18 +1202,18 @@
         <v>1</v>
       </c>
       <c r="F21" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="G21" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="G21" s="4" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="22" spans="1:9" ht="27" x14ac:dyDescent="0.3">
       <c r="A22" s="5">
         <v>45707</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>15</v>
@@ -1199,18 +1225,18 @@
         <v>2</v>
       </c>
       <c r="F22" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="G22" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="G22" s="4" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="5">
         <v>45707</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>15</v>
@@ -1222,18 +1248,18 @@
         <v>3</v>
       </c>
       <c r="F23" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="G23" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="G23" s="4" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="5">
         <v>45707</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>15</v>
@@ -1245,18 +1271,18 @@
         <v>1</v>
       </c>
       <c r="F24" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="G24" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="G24" s="4" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+    </row>
+    <row r="25" spans="1:9" ht="66.599999999999994" x14ac:dyDescent="0.3">
       <c r="A25" s="5">
         <v>45707</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>15</v>
@@ -1268,16 +1294,16 @@
         <v>1</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G25" s="4"/>
     </row>
-    <row r="26" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" ht="27" x14ac:dyDescent="0.3">
       <c r="A26" s="5">
         <v>45707</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>15</v>
@@ -1289,18 +1315,18 @@
         <v>2</v>
       </c>
       <c r="F26" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="G26" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="G26" s="4" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="27" spans="1:9" ht="27" x14ac:dyDescent="0.3">
       <c r="A27" s="5">
         <v>45709</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>15</v>
@@ -1313,15 +1339,15 @@
       </c>
       <c r="F27" s="4"/>
       <c r="G27" s="4" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="40.200000000000003" x14ac:dyDescent="0.3">
       <c r="A28" s="5">
         <v>45709</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>15</v>
@@ -1333,18 +1359,18 @@
         <v>1</v>
       </c>
       <c r="F28" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="G28" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="G28" s="4" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" s="5">
         <v>45715</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>15</v>
@@ -1358,12 +1384,12 @@
       <c r="F29" s="4"/>
       <c r="G29" s="4"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" s="5">
         <v>45715</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C30" s="4" t="s">
         <v>15</v>
@@ -1375,36 +1401,70 @@
         <v>0.3</v>
       </c>
       <c r="F30" s="4"/>
-      <c r="G30" s="4"/>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A31" s="5"/>
-      <c r="B31" s="4"/>
-      <c r="C31" s="4"/>
-      <c r="D31" s="4"/>
-      <c r="E31" s="4"/>
-      <c r="F31" s="4"/>
-      <c r="G31" s="4"/>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A32" s="4"/>
-      <c r="B32" s="4"/>
-      <c r="C32" s="4"/>
-      <c r="D32" s="4"/>
-      <c r="E32" s="4"/>
+      <c r="G30" s="4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="27" x14ac:dyDescent="0.3">
+      <c r="A31" s="5">
+        <v>45722</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E31" s="4">
+        <v>1</v>
+      </c>
+      <c r="F31" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="G31" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="27" x14ac:dyDescent="0.3">
+      <c r="A32" s="5">
+        <v>45722</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E32" s="4">
+        <v>0.3</v>
+      </c>
       <c r="F32" s="4"/>
-      <c r="G32" s="4"/>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A33" s="4"/>
+      <c r="G32" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="H32" s="6"/>
+      <c r="I32" s="6"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A33" s="5">
+        <v>45723</v>
+      </c>
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
       <c r="D33" s="4"/>
       <c r="E33" s="4"/>
       <c r="F33" s="4"/>
       <c r="G33" s="4"/>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H33" s="6"/>
+      <c r="I33" s="6"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" s="4"/>
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
@@ -1412,8 +1472,10 @@
       <c r="E34" s="4"/>
       <c r="F34" s="4"/>
       <c r="G34" s="4"/>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H34" s="6"/>
+      <c r="I34" s="6"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" s="4"/>
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
@@ -1421,42 +1483,195 @@
       <c r="E35" s="4"/>
       <c r="F35" s="4"/>
       <c r="G35" s="4"/>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A36" s="6"/>
-      <c r="B36" s="6"/>
-      <c r="C36" s="6"/>
-      <c r="D36" s="6"/>
-      <c r="E36" s="6"/>
-      <c r="F36" s="6"/>
-      <c r="G36" s="6"/>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A37" s="6"/>
-      <c r="B37" s="6"/>
-      <c r="C37" s="6"/>
-      <c r="D37" s="6"/>
-      <c r="E37" s="6"/>
-      <c r="F37" s="6"/>
-      <c r="G37" s="6"/>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A38" s="6"/>
-      <c r="B38" s="6"/>
-      <c r="C38" s="6"/>
-      <c r="D38" s="6"/>
-      <c r="E38" s="6"/>
-      <c r="F38" s="6"/>
-      <c r="G38" s="6"/>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A39" s="6"/>
-      <c r="B39" s="6"/>
-      <c r="C39" s="6"/>
-      <c r="D39" s="6"/>
-      <c r="E39" s="6"/>
-      <c r="F39" s="6"/>
-      <c r="G39" s="6"/>
+      <c r="H35" s="6"/>
+      <c r="I35" s="6"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A36" s="7"/>
+      <c r="B36" s="7"/>
+      <c r="C36" s="7"/>
+      <c r="D36" s="7"/>
+      <c r="E36" s="7"/>
+      <c r="F36" s="7"/>
+      <c r="G36" s="7"/>
+      <c r="H36" s="6"/>
+      <c r="I36" s="6"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A37" s="7"/>
+      <c r="B37" s="7"/>
+      <c r="C37" s="7"/>
+      <c r="D37" s="7"/>
+      <c r="E37" s="7"/>
+      <c r="F37" s="7"/>
+      <c r="G37" s="7"/>
+      <c r="H37" s="6"/>
+      <c r="I37" s="6"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A38" s="7"/>
+      <c r="B38" s="7"/>
+      <c r="C38" s="7"/>
+      <c r="D38" s="7"/>
+      <c r="E38" s="7"/>
+      <c r="F38" s="7"/>
+      <c r="G38" s="7"/>
+      <c r="H38" s="6"/>
+      <c r="I38" s="6"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A39" s="7"/>
+      <c r="B39" s="7"/>
+      <c r="C39" s="7"/>
+      <c r="D39" s="7"/>
+      <c r="E39" s="7"/>
+      <c r="F39" s="7"/>
+      <c r="G39" s="7"/>
+      <c r="H39" s="6"/>
+      <c r="I39" s="6"/>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A40" s="6"/>
+      <c r="B40" s="6"/>
+      <c r="C40" s="6"/>
+      <c r="D40" s="6"/>
+      <c r="E40" s="6"/>
+      <c r="F40" s="6"/>
+      <c r="G40" s="6"/>
+      <c r="H40" s="6"/>
+      <c r="I40" s="6"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A41" s="6"/>
+      <c r="B41" s="6"/>
+      <c r="C41" s="6"/>
+      <c r="D41" s="6"/>
+      <c r="E41" s="6"/>
+      <c r="F41" s="6"/>
+      <c r="G41" s="6"/>
+      <c r="H41" s="6"/>
+      <c r="I41" s="6"/>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A42" s="6"/>
+      <c r="B42" s="6"/>
+      <c r="C42" s="6"/>
+      <c r="D42" s="6"/>
+      <c r="E42" s="6"/>
+      <c r="F42" s="6"/>
+      <c r="G42" s="6"/>
+      <c r="H42" s="6"/>
+      <c r="I42" s="6"/>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A43" s="6"/>
+      <c r="B43" s="6"/>
+      <c r="C43" s="6"/>
+      <c r="D43" s="6"/>
+      <c r="E43" s="6"/>
+      <c r="F43" s="6"/>
+      <c r="G43" s="6"/>
+      <c r="H43" s="6"/>
+      <c r="I43" s="6"/>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A44" s="6"/>
+      <c r="B44" s="6"/>
+      <c r="C44" s="6"/>
+      <c r="D44" s="6"/>
+      <c r="E44" s="6"/>
+      <c r="F44" s="6"/>
+      <c r="G44" s="6"/>
+      <c r="H44" s="6"/>
+      <c r="I44" s="6"/>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A45" s="6"/>
+      <c r="B45" s="6"/>
+      <c r="C45" s="6"/>
+      <c r="D45" s="6"/>
+      <c r="E45" s="6"/>
+      <c r="F45" s="6"/>
+      <c r="G45" s="6"/>
+      <c r="H45" s="6"/>
+      <c r="I45" s="6"/>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A46" s="6"/>
+      <c r="B46" s="6"/>
+      <c r="C46" s="6"/>
+      <c r="D46" s="6"/>
+      <c r="E46" s="6"/>
+      <c r="F46" s="6"/>
+      <c r="G46" s="6"/>
+      <c r="H46" s="6"/>
+      <c r="I46" s="6"/>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A47" s="6"/>
+      <c r="B47" s="6"/>
+      <c r="C47" s="6"/>
+      <c r="D47" s="6"/>
+      <c r="E47" s="6"/>
+      <c r="F47" s="6"/>
+      <c r="G47" s="6"/>
+      <c r="H47" s="6"/>
+      <c r="I47" s="6"/>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A48" s="6"/>
+      <c r="B48" s="6"/>
+      <c r="C48" s="6"/>
+      <c r="D48" s="6"/>
+      <c r="E48" s="6"/>
+      <c r="F48" s="6"/>
+      <c r="G48" s="6"/>
+      <c r="H48" s="6"/>
+      <c r="I48" s="6"/>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A49" s="6"/>
+      <c r="B49" s="6"/>
+      <c r="C49" s="6"/>
+      <c r="D49" s="6"/>
+      <c r="E49" s="6"/>
+      <c r="F49" s="6"/>
+      <c r="G49" s="6"/>
+      <c r="H49" s="6"/>
+      <c r="I49" s="6"/>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A50" s="6"/>
+      <c r="B50" s="6"/>
+      <c r="C50" s="6"/>
+      <c r="D50" s="6"/>
+      <c r="E50" s="6"/>
+      <c r="F50" s="6"/>
+      <c r="G50" s="6"/>
+      <c r="H50" s="6"/>
+      <c r="I50" s="6"/>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A51" s="6"/>
+      <c r="B51" s="6"/>
+      <c r="C51" s="6"/>
+      <c r="D51" s="6"/>
+      <c r="E51" s="6"/>
+      <c r="F51" s="6"/>
+      <c r="G51" s="6"/>
+      <c r="H51" s="6"/>
+      <c r="I51" s="6"/>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A52" s="6"/>
+      <c r="B52" s="6"/>
+      <c r="C52" s="6"/>
+      <c r="D52" s="6"/>
+      <c r="E52" s="6"/>
+      <c r="F52" s="6"/>
+      <c r="G52" s="6"/>
+      <c r="H52" s="6"/>
+      <c r="I52" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Log updated, No Code model started, dataset added for sentimental analysis
</commit_message>
<xml_diff>
--- a/DetailedLog.xlsx
+++ b/DetailedLog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tomas\4thYearSofDev\DataScience\DataScienceModuleGitHub2\DataScienceModule\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8662133C-A9AE-4DC1-B126-4F498B1EDBAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E080619-25EA-4671-A231-0B2DFB7EA93D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{F649E3DD-3891-45EF-9659-861F4028E8C6}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{F649E3DD-3891-45EF-9659-861F4028E8C6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="97">
   <si>
     <t>Date</t>
   </si>
@@ -315,13 +315,25 @@
   </si>
   <si>
     <t>Simple model trained with FFNN using all the data</t>
+  </si>
+  <si>
+    <t>Starting ChatGPT CNN model</t>
+  </si>
+  <si>
+    <t>Only uploaded 4 images and reached the image data limit</t>
+  </si>
+  <si>
+    <t>Change model to tabular data</t>
+  </si>
+  <si>
+    <t>FFNN model for word sentimental annalysis</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -348,6 +360,16 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Ariel"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Ariel"/>
     </font>
   </fonts>
   <fills count="2">
@@ -385,7 +407,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -403,8 +425,20 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -740,13 +774,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46F8E825-9A85-45B3-9061-C505070C3A75}">
-  <dimension ref="A1:I52"/>
+  <dimension ref="A1:I64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="14.77734375" customWidth="1"/>
     <col min="2" max="2" width="55.88671875" customWidth="1"/>
@@ -757,7 +791,7 @@
     <col min="7" max="7" width="35.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="27.6" thickBot="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -780,7 +814,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" ht="15" thickBot="1">
       <c r="A2" s="2">
         <v>45674</v>
       </c>
@@ -803,7 +837,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" ht="15" thickBot="1">
       <c r="A3" s="2">
         <v>45674</v>
       </c>
@@ -826,7 +860,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="54" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" ht="54" thickBot="1">
       <c r="A4" s="2">
         <v>45674</v>
       </c>
@@ -849,7 +883,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" ht="27.6" thickBot="1">
       <c r="A5" s="2">
         <v>45675</v>
       </c>
@@ -872,7 +906,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" ht="27.6" thickBot="1">
       <c r="A6" s="2">
         <v>45680</v>
       </c>
@@ -895,7 +929,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" ht="15" thickBot="1">
       <c r="A7" s="2">
         <v>45680</v>
       </c>
@@ -918,7 +952,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" ht="40.799999999999997" thickBot="1">
       <c r="A8" s="2">
         <v>45680</v>
       </c>
@@ -941,7 +975,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" ht="15" thickBot="1">
       <c r="A9" s="2">
         <v>45680</v>
       </c>
@@ -962,7 +996,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" ht="15" thickBot="1">
       <c r="A10" s="2">
         <v>45683</v>
       </c>
@@ -985,7 +1019,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="27" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" ht="27">
       <c r="A11" s="5">
         <v>45688</v>
       </c>
@@ -1008,7 +1042,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="27" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" ht="27">
       <c r="A12" s="5">
         <v>45691</v>
       </c>
@@ -1031,7 +1065,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7">
       <c r="A13" s="5">
         <v>45691</v>
       </c>
@@ -1046,7 +1080,7 @@
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
     </row>
-    <row r="14" spans="1:7" ht="27" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" ht="27">
       <c r="A14" s="5">
         <v>45694</v>
       </c>
@@ -1069,7 +1103,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="27" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" ht="27">
       <c r="A15" s="5">
         <v>45695</v>
       </c>
@@ -1088,7 +1122,7 @@
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
     </row>
-    <row r="16" spans="1:7" ht="40.200000000000003" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" ht="40.200000000000003">
       <c r="A16" s="5">
         <v>45702</v>
       </c>
@@ -1109,7 +1143,7 @@
       </c>
       <c r="G16" s="4"/>
     </row>
-    <row r="17" spans="1:9" ht="27" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" ht="27">
       <c r="A17" s="5">
         <v>45703</v>
       </c>
@@ -1130,7 +1164,7 @@
       </c>
       <c r="G17" s="4"/>
     </row>
-    <row r="18" spans="1:9" ht="27" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" ht="27">
       <c r="A18" s="5">
         <v>45703</v>
       </c>
@@ -1151,7 +1185,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="53.4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" ht="53.4">
       <c r="A19" s="5">
         <v>45706</v>
       </c>
@@ -1174,7 +1208,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9">
       <c r="A20" s="5">
         <v>45706</v>
       </c>
@@ -1197,7 +1231,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="40.200000000000003" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" ht="40.200000000000003">
       <c r="A21" s="5">
         <v>45706</v>
       </c>
@@ -1220,7 +1254,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="27" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" ht="27">
       <c r="A22" s="5">
         <v>45707</v>
       </c>
@@ -1243,7 +1277,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9">
       <c r="A23" s="5">
         <v>45707</v>
       </c>
@@ -1266,7 +1300,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9">
       <c r="A24" s="5">
         <v>45707</v>
       </c>
@@ -1289,7 +1323,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="66.599999999999994" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" ht="66.599999999999994">
       <c r="A25" s="5">
         <v>45707</v>
       </c>
@@ -1310,7 +1344,7 @@
       </c>
       <c r="G25" s="4"/>
     </row>
-    <row r="26" spans="1:9" ht="27" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" ht="27">
       <c r="A26" s="5">
         <v>45707</v>
       </c>
@@ -1333,7 +1367,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="27" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" ht="27">
       <c r="A27" s="5">
         <v>45709</v>
       </c>
@@ -1354,7 +1388,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="40.200000000000003" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" ht="40.200000000000003">
       <c r="A28" s="5">
         <v>45709</v>
       </c>
@@ -1377,7 +1411,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9">
       <c r="A29" s="5">
         <v>45715</v>
       </c>
@@ -1396,7 +1430,7 @@
       <c r="F29" s="4"/>
       <c r="G29" s="4"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9">
       <c r="A30" s="5">
         <v>45715</v>
       </c>
@@ -1417,7 +1451,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="27" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" ht="27">
       <c r="A31" s="5">
         <v>45722</v>
       </c>
@@ -1440,7 +1474,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="27" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" ht="27">
       <c r="A32" s="5">
         <v>45722</v>
       </c>
@@ -1463,7 +1497,7 @@
       <c r="H32" s="6"/>
       <c r="I32" s="6"/>
     </row>
-    <row r="33" spans="1:9" ht="40.200000000000003" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" ht="40.200000000000003">
       <c r="A33" s="5">
         <v>45723</v>
       </c>
@@ -1488,7 +1522,7 @@
       <c r="H33" s="6"/>
       <c r="I33" s="6"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9">
       <c r="A34" s="5">
         <v>45730</v>
       </c>
@@ -1509,7 +1543,7 @@
       <c r="H34" s="6"/>
       <c r="I34" s="6"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9">
       <c r="A35" s="5">
         <v>45731</v>
       </c>
@@ -1522,192 +1556,322 @@
       <c r="H35" s="6"/>
       <c r="I35" s="6"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A36" s="7"/>
-      <c r="B36" s="7"/>
-      <c r="C36" s="7"/>
-      <c r="D36" s="7"/>
-      <c r="E36" s="7"/>
-      <c r="F36" s="7"/>
-      <c r="G36" s="7"/>
+    <row r="36" spans="1:9" ht="27">
+      <c r="A36" s="7">
+        <v>45736</v>
+      </c>
+      <c r="B36" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="C36" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D36" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E36" s="8">
+        <v>0.3</v>
+      </c>
+      <c r="F36" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="G36" s="8" t="s">
+        <v>95</v>
+      </c>
       <c r="H36" s="6"/>
       <c r="I36" s="6"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A37" s="7"/>
-      <c r="B37" s="7"/>
-      <c r="C37" s="7"/>
-      <c r="D37" s="7"/>
-      <c r="E37" s="7"/>
-      <c r="F37" s="7"/>
-      <c r="G37" s="7"/>
+    <row r="37" spans="1:9">
+      <c r="A37" s="7">
+        <v>45736</v>
+      </c>
+      <c r="B37" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="C37" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D37" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E37" s="8"/>
+      <c r="F37" s="8"/>
+      <c r="G37" s="8"/>
       <c r="H37" s="6"/>
       <c r="I37" s="6"/>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A38" s="7"/>
-      <c r="B38" s="7"/>
-      <c r="C38" s="7"/>
-      <c r="D38" s="7"/>
-      <c r="E38" s="7"/>
-      <c r="F38" s="7"/>
-      <c r="G38" s="7"/>
+    <row r="38" spans="1:9">
+      <c r="A38" s="8"/>
+      <c r="B38" s="8"/>
+      <c r="C38" s="8"/>
+      <c r="D38" s="8"/>
+      <c r="E38" s="8"/>
+      <c r="F38" s="8"/>
+      <c r="G38" s="8"/>
       <c r="H38" s="6"/>
       <c r="I38" s="6"/>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A39" s="7"/>
-      <c r="B39" s="7"/>
-      <c r="C39" s="7"/>
-      <c r="D39" s="7"/>
-      <c r="E39" s="7"/>
-      <c r="F39" s="7"/>
-      <c r="G39" s="7"/>
+    <row r="39" spans="1:9">
+      <c r="A39" s="8"/>
+      <c r="B39" s="8"/>
+      <c r="C39" s="8"/>
+      <c r="D39" s="8"/>
+      <c r="E39" s="8"/>
+      <c r="F39" s="8"/>
+      <c r="G39" s="8"/>
       <c r="H39" s="6"/>
       <c r="I39" s="6"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A40" s="6"/>
-      <c r="B40" s="6"/>
-      <c r="C40" s="6"/>
-      <c r="D40" s="6"/>
-      <c r="E40" s="6"/>
-      <c r="F40" s="6"/>
-      <c r="G40" s="6"/>
+    <row r="40" spans="1:9">
+      <c r="A40" s="9"/>
+      <c r="B40" s="9"/>
+      <c r="C40" s="9"/>
+      <c r="D40" s="9"/>
+      <c r="E40" s="9"/>
+      <c r="F40" s="9"/>
+      <c r="G40" s="9"/>
       <c r="H40" s="6"/>
       <c r="I40" s="6"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A41" s="6"/>
-      <c r="B41" s="6"/>
-      <c r="C41" s="6"/>
-      <c r="D41" s="6"/>
-      <c r="E41" s="6"/>
-      <c r="F41" s="6"/>
-      <c r="G41" s="6"/>
+    <row r="41" spans="1:9">
+      <c r="A41" s="9"/>
+      <c r="B41" s="9"/>
+      <c r="C41" s="9"/>
+      <c r="D41" s="9"/>
+      <c r="E41" s="9"/>
+      <c r="F41" s="9"/>
+      <c r="G41" s="9"/>
       <c r="H41" s="6"/>
       <c r="I41" s="6"/>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A42" s="6"/>
-      <c r="B42" s="6"/>
-      <c r="C42" s="6"/>
-      <c r="D42" s="6"/>
-      <c r="E42" s="6"/>
-      <c r="F42" s="6"/>
-      <c r="G42" s="6"/>
+    <row r="42" spans="1:9">
+      <c r="A42" s="9"/>
+      <c r="B42" s="9"/>
+      <c r="C42" s="9"/>
+      <c r="D42" s="9"/>
+      <c r="E42" s="9"/>
+      <c r="F42" s="9"/>
+      <c r="G42" s="9"/>
       <c r="H42" s="6"/>
       <c r="I42" s="6"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A43" s="6"/>
-      <c r="B43" s="6"/>
-      <c r="C43" s="6"/>
-      <c r="D43" s="6"/>
-      <c r="E43" s="6"/>
-      <c r="F43" s="6"/>
-      <c r="G43" s="6"/>
+    <row r="43" spans="1:9">
+      <c r="A43" s="9"/>
+      <c r="B43" s="9"/>
+      <c r="C43" s="9"/>
+      <c r="D43" s="9"/>
+      <c r="E43" s="9"/>
+      <c r="F43" s="9"/>
+      <c r="G43" s="9"/>
       <c r="H43" s="6"/>
       <c r="I43" s="6"/>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A44" s="6"/>
-      <c r="B44" s="6"/>
-      <c r="C44" s="6"/>
-      <c r="D44" s="6"/>
-      <c r="E44" s="6"/>
-      <c r="F44" s="6"/>
-      <c r="G44" s="6"/>
+    <row r="44" spans="1:9">
+      <c r="A44" s="9"/>
+      <c r="B44" s="9"/>
+      <c r="C44" s="9"/>
+      <c r="D44" s="9"/>
+      <c r="E44" s="9"/>
+      <c r="F44" s="9"/>
+      <c r="G44" s="9"/>
       <c r="H44" s="6"/>
       <c r="I44" s="6"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A45" s="6"/>
-      <c r="B45" s="6"/>
-      <c r="C45" s="6"/>
-      <c r="D45" s="6"/>
-      <c r="E45" s="6"/>
-      <c r="F45" s="6"/>
-      <c r="G45" s="6"/>
+    <row r="45" spans="1:9">
+      <c r="A45" s="9"/>
+      <c r="B45" s="9"/>
+      <c r="C45" s="9"/>
+      <c r="D45" s="9"/>
+      <c r="E45" s="9"/>
+      <c r="F45" s="9"/>
+      <c r="G45" s="9"/>
       <c r="H45" s="6"/>
       <c r="I45" s="6"/>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A46" s="6"/>
-      <c r="B46" s="6"/>
-      <c r="C46" s="6"/>
-      <c r="D46" s="6"/>
-      <c r="E46" s="6"/>
-      <c r="F46" s="6"/>
-      <c r="G46" s="6"/>
+    <row r="46" spans="1:9">
+      <c r="A46" s="9"/>
+      <c r="B46" s="9"/>
+      <c r="C46" s="9"/>
+      <c r="D46" s="9"/>
+      <c r="E46" s="9"/>
+      <c r="F46" s="9"/>
+      <c r="G46" s="9"/>
       <c r="H46" s="6"/>
       <c r="I46" s="6"/>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A47" s="6"/>
-      <c r="B47" s="6"/>
-      <c r="C47" s="6"/>
-      <c r="D47" s="6"/>
-      <c r="E47" s="6"/>
-      <c r="F47" s="6"/>
-      <c r="G47" s="6"/>
+    <row r="47" spans="1:9">
+      <c r="A47" s="9"/>
+      <c r="B47" s="9"/>
+      <c r="C47" s="9"/>
+      <c r="D47" s="9"/>
+      <c r="E47" s="9"/>
+      <c r="F47" s="9"/>
+      <c r="G47" s="9"/>
       <c r="H47" s="6"/>
       <c r="I47" s="6"/>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A48" s="6"/>
-      <c r="B48" s="6"/>
-      <c r="C48" s="6"/>
-      <c r="D48" s="6"/>
-      <c r="E48" s="6"/>
-      <c r="F48" s="6"/>
-      <c r="G48" s="6"/>
+    <row r="48" spans="1:9">
+      <c r="A48" s="9"/>
+      <c r="B48" s="9"/>
+      <c r="C48" s="9"/>
+      <c r="D48" s="9"/>
+      <c r="E48" s="9"/>
+      <c r="F48" s="9"/>
+      <c r="G48" s="9"/>
       <c r="H48" s="6"/>
       <c r="I48" s="6"/>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A49" s="6"/>
-      <c r="B49" s="6"/>
-      <c r="C49" s="6"/>
-      <c r="D49" s="6"/>
-      <c r="E49" s="6"/>
-      <c r="F49" s="6"/>
-      <c r="G49" s="6"/>
+    <row r="49" spans="1:9">
+      <c r="A49" s="9"/>
+      <c r="B49" s="9"/>
+      <c r="C49" s="9"/>
+      <c r="D49" s="9"/>
+      <c r="E49" s="9"/>
+      <c r="F49" s="9"/>
+      <c r="G49" s="9"/>
       <c r="H49" s="6"/>
       <c r="I49" s="6"/>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A50" s="6"/>
-      <c r="B50" s="6"/>
-      <c r="C50" s="6"/>
-      <c r="D50" s="6"/>
-      <c r="E50" s="6"/>
-      <c r="F50" s="6"/>
-      <c r="G50" s="6"/>
+    <row r="50" spans="1:9">
+      <c r="A50" s="9"/>
+      <c r="B50" s="9"/>
+      <c r="C50" s="9"/>
+      <c r="D50" s="9"/>
+      <c r="E50" s="9"/>
+      <c r="F50" s="9"/>
+      <c r="G50" s="9"/>
       <c r="H50" s="6"/>
       <c r="I50" s="6"/>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A51" s="6"/>
-      <c r="B51" s="6"/>
-      <c r="C51" s="6"/>
-      <c r="D51" s="6"/>
-      <c r="E51" s="6"/>
-      <c r="F51" s="6"/>
-      <c r="G51" s="6"/>
+    <row r="51" spans="1:9">
+      <c r="A51" s="9"/>
+      <c r="B51" s="9"/>
+      <c r="C51" s="9"/>
+      <c r="D51" s="9"/>
+      <c r="E51" s="9"/>
+      <c r="F51" s="9"/>
+      <c r="G51" s="9"/>
       <c r="H51" s="6"/>
       <c r="I51" s="6"/>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A52" s="6"/>
-      <c r="B52" s="6"/>
-      <c r="C52" s="6"/>
-      <c r="D52" s="6"/>
-      <c r="E52" s="6"/>
-      <c r="F52" s="6"/>
-      <c r="G52" s="6"/>
+    <row r="52" spans="1:9">
+      <c r="A52" s="9"/>
+      <c r="B52" s="9"/>
+      <c r="C52" s="9"/>
+      <c r="D52" s="9"/>
+      <c r="E52" s="9"/>
+      <c r="F52" s="9"/>
+      <c r="G52" s="9"/>
       <c r="H52" s="6"/>
       <c r="I52" s="6"/>
+    </row>
+    <row r="53" spans="1:9">
+      <c r="A53" s="10"/>
+      <c r="B53" s="10"/>
+      <c r="C53" s="10"/>
+      <c r="D53" s="10"/>
+      <c r="E53" s="10"/>
+      <c r="F53" s="10"/>
+      <c r="G53" s="10"/>
+    </row>
+    <row r="54" spans="1:9">
+      <c r="A54" s="10"/>
+      <c r="B54" s="10"/>
+      <c r="C54" s="10"/>
+      <c r="D54" s="10"/>
+      <c r="E54" s="10"/>
+      <c r="F54" s="10"/>
+      <c r="G54" s="10"/>
+    </row>
+    <row r="55" spans="1:9">
+      <c r="A55" s="10"/>
+      <c r="B55" s="10"/>
+      <c r="C55" s="10"/>
+      <c r="D55" s="10"/>
+      <c r="E55" s="10"/>
+      <c r="F55" s="10"/>
+      <c r="G55" s="10"/>
+    </row>
+    <row r="56" spans="1:9">
+      <c r="A56" s="10"/>
+      <c r="B56" s="10"/>
+      <c r="C56" s="10"/>
+      <c r="D56" s="10"/>
+      <c r="E56" s="10"/>
+      <c r="F56" s="10"/>
+      <c r="G56" s="10"/>
+    </row>
+    <row r="57" spans="1:9">
+      <c r="A57" s="10"/>
+      <c r="B57" s="10"/>
+      <c r="C57" s="10"/>
+      <c r="D57" s="10"/>
+      <c r="E57" s="10"/>
+      <c r="F57" s="10"/>
+      <c r="G57" s="10"/>
+    </row>
+    <row r="58" spans="1:9">
+      <c r="A58" s="10"/>
+      <c r="B58" s="10"/>
+      <c r="C58" s="10"/>
+      <c r="D58" s="10"/>
+      <c r="E58" s="10"/>
+      <c r="F58" s="10"/>
+      <c r="G58" s="10"/>
+    </row>
+    <row r="59" spans="1:9">
+      <c r="A59" s="10"/>
+      <c r="B59" s="10"/>
+      <c r="C59" s="10"/>
+      <c r="D59" s="10"/>
+      <c r="E59" s="10"/>
+      <c r="F59" s="10"/>
+      <c r="G59" s="10"/>
+    </row>
+    <row r="60" spans="1:9">
+      <c r="A60" s="10"/>
+      <c r="B60" s="10"/>
+      <c r="C60" s="10"/>
+      <c r="D60" s="10"/>
+      <c r="E60" s="10"/>
+      <c r="F60" s="10"/>
+      <c r="G60" s="10"/>
+    </row>
+    <row r="61" spans="1:9">
+      <c r="A61" s="10"/>
+      <c r="B61" s="10"/>
+      <c r="C61" s="10"/>
+      <c r="D61" s="10"/>
+      <c r="E61" s="10"/>
+      <c r="F61" s="10"/>
+      <c r="G61" s="10"/>
+    </row>
+    <row r="62" spans="1:9">
+      <c r="A62" s="10"/>
+      <c r="B62" s="10"/>
+      <c r="C62" s="10"/>
+      <c r="D62" s="10"/>
+      <c r="E62" s="10"/>
+      <c r="F62" s="10"/>
+      <c r="G62" s="10"/>
+    </row>
+    <row r="63" spans="1:9">
+      <c r="A63" s="10"/>
+      <c r="B63" s="10"/>
+      <c r="C63" s="10"/>
+      <c r="D63" s="10"/>
+      <c r="E63" s="10"/>
+      <c r="F63" s="10"/>
+      <c r="G63" s="10"/>
+    </row>
+    <row r="64" spans="1:9">
+      <c r="A64" s="11"/>
+      <c r="B64" s="11"/>
+      <c r="C64" s="11"/>
+      <c r="D64" s="11"/>
+      <c r="E64" s="11"/>
+      <c r="F64" s="11"/>
+      <c r="G64" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Log updated, images added for chatGPT code generation
</commit_message>
<xml_diff>
--- a/DetailedLog.xlsx
+++ b/DetailedLog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tomas\4thYearSofDev\DataScience\DataScienceModuleGitHub2\DataScienceModule\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9CE69B5-F3F3-4B18-A06A-8D1C1B095D80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B530F3E4-29FC-4575-AA48-9BD5998D4007}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{F649E3DD-3891-45EF-9659-861F4028E8C6}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="106">
   <si>
     <t>Date</t>
   </si>
@@ -336,6 +336,24 @@
   </si>
   <si>
     <t>FFNN model for word sentimental annalysis smaller dataset</t>
+  </si>
+  <si>
+    <t>Gives code to train the model but does not do it for you</t>
+  </si>
+  <si>
+    <t>Try it on DeepSeek</t>
+  </si>
+  <si>
+    <t>Trying to train a NN model on Deepseek</t>
+  </si>
+  <si>
+    <t>Same issue as chatGPT, give you code to train it but dosnt do it for you</t>
+  </si>
+  <si>
+    <t>Try both chatGPT and DeepSeek code in colab</t>
+  </si>
+  <si>
+    <t>Trying chatGPT and DeepSeek generated code</t>
   </si>
 </sst>
 </file>
@@ -440,14 +458,14 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -785,8 +803,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46F8E825-9A85-45B3-9061-C505070C3A75}">
   <dimension ref="A1:I64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="F42" sqref="F42"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="F43" sqref="F43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1615,7 +1633,7 @@
       <c r="H37" s="6"/>
       <c r="I37" s="6"/>
     </row>
-    <row r="38" spans="1:9">
+    <row r="38" spans="1:9" ht="27">
       <c r="A38" s="7">
         <v>45736</v>
       </c>
@@ -1628,273 +1646,303 @@
       <c r="D38" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="E38" s="8"/>
-      <c r="F38" s="8"/>
-      <c r="G38" s="8"/>
+      <c r="E38" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="F38" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="G38" s="8" t="s">
+        <v>101</v>
+      </c>
       <c r="H38" s="6"/>
       <c r="I38" s="6"/>
     </row>
-    <row r="39" spans="1:9">
-      <c r="A39" s="8"/>
-      <c r="B39" s="8"/>
-      <c r="C39" s="8"/>
-      <c r="D39" s="8"/>
-      <c r="E39" s="8"/>
-      <c r="F39" s="8"/>
-      <c r="G39" s="8"/>
+    <row r="39" spans="1:9" ht="40.200000000000003">
+      <c r="A39" s="7">
+        <v>45736</v>
+      </c>
+      <c r="B39" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="C39" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D39" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E39" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="F39" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="G39" s="8" t="s">
+        <v>104</v>
+      </c>
       <c r="H39" s="6"/>
       <c r="I39" s="6"/>
     </row>
     <row r="40" spans="1:9">
-      <c r="A40" s="9"/>
-      <c r="B40" s="9"/>
-      <c r="C40" s="9"/>
-      <c r="D40" s="9"/>
-      <c r="E40" s="9"/>
-      <c r="F40" s="9"/>
-      <c r="G40" s="9"/>
+      <c r="A40" s="7">
+        <v>45736</v>
+      </c>
+      <c r="B40" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="C40" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D40" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E40" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="F40" s="8"/>
+      <c r="G40" s="8"/>
       <c r="H40" s="6"/>
       <c r="I40" s="6"/>
     </row>
     <row r="41" spans="1:9">
-      <c r="A41" s="9"/>
-      <c r="B41" s="9"/>
-      <c r="C41" s="9"/>
-      <c r="D41" s="9"/>
-      <c r="E41" s="9"/>
-      <c r="F41" s="9"/>
-      <c r="G41" s="9"/>
+      <c r="A41" s="8"/>
+      <c r="B41" s="8"/>
+      <c r="C41" s="8"/>
+      <c r="D41" s="8"/>
+      <c r="E41" s="8"/>
+      <c r="F41" s="8"/>
+      <c r="G41" s="8"/>
       <c r="H41" s="6"/>
       <c r="I41" s="6"/>
     </row>
     <row r="42" spans="1:9">
-      <c r="A42" s="9"/>
-      <c r="B42" s="9"/>
-      <c r="C42" s="9"/>
-      <c r="D42" s="9"/>
-      <c r="E42" s="9"/>
-      <c r="F42" s="9"/>
-      <c r="G42" s="9"/>
+      <c r="A42" s="8"/>
+      <c r="B42" s="8"/>
+      <c r="C42" s="8"/>
+      <c r="D42" s="8"/>
+      <c r="E42" s="8"/>
+      <c r="F42" s="8"/>
+      <c r="G42" s="8"/>
       <c r="H42" s="6"/>
       <c r="I42" s="6"/>
     </row>
     <row r="43" spans="1:9">
-      <c r="A43" s="9"/>
-      <c r="B43" s="9"/>
-      <c r="C43" s="9"/>
-      <c r="D43" s="9"/>
-      <c r="E43" s="9"/>
-      <c r="F43" s="9"/>
-      <c r="G43" s="9"/>
+      <c r="A43" s="8"/>
+      <c r="B43" s="8"/>
+      <c r="C43" s="8"/>
+      <c r="D43" s="8"/>
+      <c r="E43" s="8"/>
+      <c r="F43" s="8"/>
+      <c r="G43" s="8"/>
       <c r="H43" s="6"/>
       <c r="I43" s="6"/>
     </row>
     <row r="44" spans="1:9">
-      <c r="A44" s="9"/>
-      <c r="B44" s="9"/>
-      <c r="C44" s="9"/>
-      <c r="D44" s="9"/>
-      <c r="E44" s="9"/>
-      <c r="F44" s="9"/>
-      <c r="G44" s="9"/>
+      <c r="A44" s="8"/>
+      <c r="B44" s="8"/>
+      <c r="C44" s="8"/>
+      <c r="D44" s="8"/>
+      <c r="E44" s="8"/>
+      <c r="F44" s="8"/>
+      <c r="G44" s="8"/>
       <c r="H44" s="6"/>
       <c r="I44" s="6"/>
     </row>
     <row r="45" spans="1:9">
-      <c r="A45" s="9"/>
-      <c r="B45" s="9"/>
-      <c r="C45" s="9"/>
-      <c r="D45" s="9"/>
-      <c r="E45" s="9"/>
-      <c r="F45" s="9"/>
-      <c r="G45" s="9"/>
+      <c r="A45" s="8"/>
+      <c r="B45" s="8"/>
+      <c r="C45" s="8"/>
+      <c r="D45" s="8"/>
+      <c r="E45" s="8"/>
+      <c r="F45" s="8"/>
+      <c r="G45" s="8"/>
       <c r="H45" s="6"/>
       <c r="I45" s="6"/>
     </row>
     <row r="46" spans="1:9">
-      <c r="A46" s="9"/>
-      <c r="B46" s="9"/>
-      <c r="C46" s="9"/>
-      <c r="D46" s="9"/>
-      <c r="E46" s="9"/>
-      <c r="F46" s="9"/>
-      <c r="G46" s="9"/>
+      <c r="A46" s="8"/>
+      <c r="B46" s="8"/>
+      <c r="C46" s="8"/>
+      <c r="D46" s="8"/>
+      <c r="E46" s="8"/>
+      <c r="F46" s="8"/>
+      <c r="G46" s="8"/>
       <c r="H46" s="6"/>
       <c r="I46" s="6"/>
     </row>
     <row r="47" spans="1:9">
-      <c r="A47" s="9"/>
-      <c r="B47" s="9"/>
-      <c r="C47" s="9"/>
-      <c r="D47" s="9"/>
-      <c r="E47" s="9"/>
-      <c r="F47" s="9"/>
-      <c r="G47" s="9"/>
+      <c r="A47" s="8"/>
+      <c r="B47" s="8"/>
+      <c r="C47" s="8"/>
+      <c r="D47" s="8"/>
+      <c r="E47" s="8"/>
+      <c r="F47" s="8"/>
+      <c r="G47" s="8"/>
       <c r="H47" s="6"/>
       <c r="I47" s="6"/>
     </row>
     <row r="48" spans="1:9">
-      <c r="A48" s="9"/>
-      <c r="B48" s="9"/>
-      <c r="C48" s="9"/>
-      <c r="D48" s="9"/>
-      <c r="E48" s="9"/>
-      <c r="F48" s="9"/>
-      <c r="G48" s="9"/>
+      <c r="A48" s="8"/>
+      <c r="B48" s="8"/>
+      <c r="C48" s="8"/>
+      <c r="D48" s="8"/>
+      <c r="E48" s="8"/>
+      <c r="F48" s="8"/>
+      <c r="G48" s="8"/>
       <c r="H48" s="6"/>
       <c r="I48" s="6"/>
     </row>
     <row r="49" spans="1:9">
-      <c r="A49" s="9"/>
-      <c r="B49" s="9"/>
-      <c r="C49" s="9"/>
-      <c r="D49" s="9"/>
-      <c r="E49" s="9"/>
-      <c r="F49" s="9"/>
-      <c r="G49" s="9"/>
+      <c r="A49" s="8"/>
+      <c r="B49" s="8"/>
+      <c r="C49" s="8"/>
+      <c r="D49" s="8"/>
+      <c r="E49" s="8"/>
+      <c r="F49" s="8"/>
+      <c r="G49" s="8"/>
       <c r="H49" s="6"/>
       <c r="I49" s="6"/>
     </row>
     <row r="50" spans="1:9">
-      <c r="A50" s="9"/>
-      <c r="B50" s="9"/>
-      <c r="C50" s="9"/>
-      <c r="D50" s="9"/>
-      <c r="E50" s="9"/>
-      <c r="F50" s="9"/>
-      <c r="G50" s="9"/>
+      <c r="A50" s="8"/>
+      <c r="B50" s="8"/>
+      <c r="C50" s="8"/>
+      <c r="D50" s="8"/>
+      <c r="E50" s="8"/>
+      <c r="F50" s="8"/>
+      <c r="G50" s="8"/>
       <c r="H50" s="6"/>
       <c r="I50" s="6"/>
     </row>
     <row r="51" spans="1:9">
-      <c r="A51" s="9"/>
-      <c r="B51" s="9"/>
-      <c r="C51" s="9"/>
-      <c r="D51" s="9"/>
-      <c r="E51" s="9"/>
-      <c r="F51" s="9"/>
-      <c r="G51" s="9"/>
+      <c r="A51" s="8"/>
+      <c r="B51" s="8"/>
+      <c r="C51" s="8"/>
+      <c r="D51" s="8"/>
+      <c r="E51" s="8"/>
+      <c r="F51" s="8"/>
+      <c r="G51" s="8"/>
       <c r="H51" s="6"/>
       <c r="I51" s="6"/>
     </row>
     <row r="52" spans="1:9">
-      <c r="A52" s="9"/>
-      <c r="B52" s="9"/>
-      <c r="C52" s="9"/>
-      <c r="D52" s="9"/>
-      <c r="E52" s="9"/>
-      <c r="F52" s="9"/>
-      <c r="G52" s="9"/>
+      <c r="A52" s="8"/>
+      <c r="B52" s="8"/>
+      <c r="C52" s="8"/>
+      <c r="D52" s="8"/>
+      <c r="E52" s="8"/>
+      <c r="F52" s="8"/>
+      <c r="G52" s="8"/>
       <c r="H52" s="6"/>
       <c r="I52" s="6"/>
     </row>
     <row r="53" spans="1:9">
-      <c r="A53" s="10"/>
-      <c r="B53" s="10"/>
-      <c r="C53" s="10"/>
-      <c r="D53" s="10"/>
-      <c r="E53" s="10"/>
-      <c r="F53" s="10"/>
-      <c r="G53" s="10"/>
+      <c r="A53" s="11"/>
+      <c r="B53" s="11"/>
+      <c r="C53" s="11"/>
+      <c r="D53" s="11"/>
+      <c r="E53" s="11"/>
+      <c r="F53" s="11"/>
+      <c r="G53" s="11"/>
     </row>
     <row r="54" spans="1:9">
-      <c r="A54" s="10"/>
-      <c r="B54" s="10"/>
-      <c r="C54" s="10"/>
-      <c r="D54" s="10"/>
-      <c r="E54" s="10"/>
-      <c r="F54" s="10"/>
-      <c r="G54" s="10"/>
+      <c r="A54" s="11"/>
+      <c r="B54" s="11"/>
+      <c r="C54" s="11"/>
+      <c r="D54" s="11"/>
+      <c r="E54" s="11"/>
+      <c r="F54" s="11"/>
+      <c r="G54" s="11"/>
     </row>
     <row r="55" spans="1:9">
-      <c r="A55" s="10"/>
-      <c r="B55" s="10"/>
-      <c r="C55" s="10"/>
-      <c r="D55" s="10"/>
-      <c r="E55" s="10"/>
-      <c r="F55" s="10"/>
-      <c r="G55" s="10"/>
+      <c r="A55" s="11"/>
+      <c r="B55" s="11"/>
+      <c r="C55" s="11"/>
+      <c r="D55" s="11"/>
+      <c r="E55" s="11"/>
+      <c r="F55" s="11"/>
+      <c r="G55" s="11"/>
     </row>
     <row r="56" spans="1:9">
-      <c r="A56" s="10"/>
-      <c r="B56" s="10"/>
-      <c r="C56" s="10"/>
-      <c r="D56" s="10"/>
-      <c r="E56" s="10"/>
-      <c r="F56" s="10"/>
-      <c r="G56" s="10"/>
+      <c r="A56" s="11"/>
+      <c r="B56" s="11"/>
+      <c r="C56" s="11"/>
+      <c r="D56" s="11"/>
+      <c r="E56" s="11"/>
+      <c r="F56" s="11"/>
+      <c r="G56" s="11"/>
     </row>
     <row r="57" spans="1:9">
-      <c r="A57" s="10"/>
-      <c r="B57" s="10"/>
-      <c r="C57" s="10"/>
-      <c r="D57" s="10"/>
-      <c r="E57" s="10"/>
-      <c r="F57" s="10"/>
-      <c r="G57" s="10"/>
+      <c r="A57" s="11"/>
+      <c r="B57" s="11"/>
+      <c r="C57" s="11"/>
+      <c r="D57" s="11"/>
+      <c r="E57" s="11"/>
+      <c r="F57" s="11"/>
+      <c r="G57" s="11"/>
     </row>
     <row r="58" spans="1:9">
-      <c r="A58" s="10"/>
-      <c r="B58" s="10"/>
-      <c r="C58" s="10"/>
-      <c r="D58" s="10"/>
-      <c r="E58" s="10"/>
-      <c r="F58" s="10"/>
-      <c r="G58" s="10"/>
+      <c r="A58" s="11"/>
+      <c r="B58" s="11"/>
+      <c r="C58" s="11"/>
+      <c r="D58" s="11"/>
+      <c r="E58" s="11"/>
+      <c r="F58" s="11"/>
+      <c r="G58" s="11"/>
     </row>
     <row r="59" spans="1:9">
-      <c r="A59" s="10"/>
-      <c r="B59" s="10"/>
-      <c r="C59" s="10"/>
-      <c r="D59" s="10"/>
-      <c r="E59" s="10"/>
-      <c r="F59" s="10"/>
-      <c r="G59" s="10"/>
+      <c r="A59" s="11"/>
+      <c r="B59" s="11"/>
+      <c r="C59" s="11"/>
+      <c r="D59" s="11"/>
+      <c r="E59" s="11"/>
+      <c r="F59" s="11"/>
+      <c r="G59" s="11"/>
     </row>
     <row r="60" spans="1:9">
-      <c r="A60" s="10"/>
-      <c r="B60" s="10"/>
-      <c r="C60" s="10"/>
-      <c r="D60" s="10"/>
-      <c r="E60" s="10"/>
-      <c r="F60" s="10"/>
-      <c r="G60" s="10"/>
+      <c r="A60" s="11"/>
+      <c r="B60" s="11"/>
+      <c r="C60" s="11"/>
+      <c r="D60" s="11"/>
+      <c r="E60" s="11"/>
+      <c r="F60" s="11"/>
+      <c r="G60" s="11"/>
     </row>
     <row r="61" spans="1:9">
-      <c r="A61" s="10"/>
-      <c r="B61" s="10"/>
-      <c r="C61" s="10"/>
-      <c r="D61" s="10"/>
-      <c r="E61" s="10"/>
-      <c r="F61" s="10"/>
-      <c r="G61" s="10"/>
+      <c r="A61" s="9"/>
+      <c r="B61" s="9"/>
+      <c r="C61" s="9"/>
+      <c r="D61" s="9"/>
+      <c r="E61" s="9"/>
+      <c r="F61" s="9"/>
+      <c r="G61" s="9"/>
     </row>
     <row r="62" spans="1:9">
-      <c r="A62" s="10"/>
-      <c r="B62" s="10"/>
-      <c r="C62" s="10"/>
-      <c r="D62" s="10"/>
-      <c r="E62" s="10"/>
-      <c r="F62" s="10"/>
-      <c r="G62" s="10"/>
+      <c r="A62" s="9"/>
+      <c r="B62" s="9"/>
+      <c r="C62" s="9"/>
+      <c r="D62" s="9"/>
+      <c r="E62" s="9"/>
+      <c r="F62" s="9"/>
+      <c r="G62" s="9"/>
     </row>
     <row r="63" spans="1:9">
-      <c r="A63" s="10"/>
-      <c r="B63" s="10"/>
-      <c r="C63" s="10"/>
-      <c r="D63" s="10"/>
-      <c r="E63" s="10"/>
-      <c r="F63" s="10"/>
-      <c r="G63" s="10"/>
+      <c r="A63" s="9"/>
+      <c r="B63" s="9"/>
+      <c r="C63" s="9"/>
+      <c r="D63" s="9"/>
+      <c r="E63" s="9"/>
+      <c r="F63" s="9"/>
+      <c r="G63" s="9"/>
     </row>
     <row r="64" spans="1:9">
-      <c r="A64" s="11"/>
-      <c r="B64" s="11"/>
-      <c r="C64" s="11"/>
-      <c r="D64" s="11"/>
-      <c r="E64" s="11"/>
-      <c r="F64" s="11"/>
-      <c r="G64" s="11"/>
+      <c r="A64" s="10"/>
+      <c r="B64" s="10"/>
+      <c r="C64" s="10"/>
+      <c r="D64" s="10"/>
+      <c r="E64" s="10"/>
+      <c r="F64" s="10"/>
+      <c r="G64" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>